<commit_message>
Improve location shortening: no ellipsis, better abbreviations
Updated LLM prompt based on user feedback to produce better results:

Before: Used ellipsis when over 50 chars
After: Aggressive abbreviations, no ellipsis, keep essential info

Key improvements:
- Use 'Lk' instead of 'Lake'
- Slash notation for intersections: CR70/SH74
- Remove city names (already in other fields)
- Remove 'intersection of', 'at', etc.
- Compress distances: '5 KM ESE' → '5KM ESE'
- NO ELLIPSIS - abbreviate instead

Example:
  Original (122 chars):
    'Round Lake Road near Tuscarora Lodge at the intersection
     of County Road 70 and State Highway 74, 5 KM ESE of
     Fredricksburg'

  Shortened (49 chars):
    'Round Lk Rd nr Tuscarora Lodge, 5KM ESE CR70/SH74'

Test result: LLM produces exact expected output ✓

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_with_errors.xlsx
+++ b/tests/fixtures/test_with_errors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\lepsox\tests\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.51.237\projects\lepsox\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C63914-0448-4DE7-BF44-E9F4B5B547E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5158C9F6-51EC-4E4E-A4BF-BD0C2555AAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30285" yWindow="2460" windowWidth="21240" windowHeight="17160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -755,15 +755,6 @@
     <t>Plouff Creek Count, incorrectly ID as  Erynnis juvenalis at Bob Richardson Campground Site 22; next to Woodman Creek; Used bait trap with UV/MV Lights.</t>
   </si>
   <si>
-    <t>Round Lake Road near Tuscarora Lodge at the intersection of County Road 70 and State Highway 74, 3 miles North of Fredricksburg</t>
-  </si>
-  <si>
-    <t>Round Lake Road near Tuscarora Lodge at the intersection of County Road 70 and State Highway 74, 5 KM East South East of Fredricksburg</t>
-  </si>
-  <si>
-    <t>Round Lake Road near Tuscarora Lodge at the intersection of County Road 70 and State Highway 74, 5 KM WSW of Fredricksburg</t>
-  </si>
-  <si>
     <t>Door</t>
   </si>
   <si>
@@ -819,6 +810,15 @@
   </si>
   <si>
     <t>EPO</t>
+  </si>
+  <si>
+    <t>BIg Lake Campground at the intersection of Hwy P and Big Lake Campground Road</t>
+  </si>
+  <si>
+    <t>Round Lake Road near Tuscarora Lodge  3 miles North of Fredricksburg on County Road 54</t>
+  </si>
+  <si>
+    <t>Dillon Dam Road  at the intersection of County Road 70 and State Highway 74, 5 KM East South East</t>
   </si>
 </sst>
 </file>
@@ -2980,25 +2980,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="5" customWidth="1"/>
-    <col min="2" max="3" width="10.875" style="5"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
+    <col min="2" max="3" width="10.84765625" style="5"/>
+    <col min="4" max="4" width="14.84765625" customWidth="1"/>
+    <col min="5" max="5" width="16.34765625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="10" max="10" width="13.125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="116.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.09765625" customWidth="1"/>
+    <col min="10" max="10" width="13.09765625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="116.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.34765625" style="5" customWidth="1"/>
     <col min="13" max="13" width="12.5" style="5" customWidth="1"/>
-    <col min="14" max="14" width="32.375" customWidth="1"/>
-    <col min="15" max="15" width="129.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="59.875" customWidth="1"/>
+    <col min="14" max="14" width="32.34765625" customWidth="1"/>
+    <col min="15" max="15" width="129.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="59.84765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3156,13 +3156,13 @@
         <v>141</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="L4" s="11">
         <v>45474</v>
@@ -3205,7 +3205,7 @@
         <v>133</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="L5" s="11">
         <v>45474</v>
@@ -3215,7 +3215,7 @@
         <v>182</v>
       </c>
       <c r="O5" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="P5">
         <v>2024</v>
@@ -3244,20 +3244,20 @@
         <v>141</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>133</v>
       </c>
       <c r="K6" s="21" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="L6" s="11">
         <v>45480</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>237</v>
@@ -3289,10 +3289,10 @@
         <v>141</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>191</v>
@@ -3302,7 +3302,7 @@
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O7" s="21" t="s">
         <v>238</v>
@@ -3347,7 +3347,7 @@
         <v>45461</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O8" t="s">
         <v>170</v>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O9" s="9" t="s">
         <v>202</v>
@@ -3416,16 +3416,16 @@
         <v>18</v>
       </c>
       <c r="F10" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>246</v>
-      </c>
       <c r="J10" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>189</v>
@@ -3435,7 +3435,7 @@
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O10" s="9" t="s">
         <v>202</v>
@@ -3464,10 +3464,10 @@
         <v>19</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="10" t="s">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O11" s="9" t="s">
         <v>197</v>
@@ -3526,7 +3526,7 @@
         <v>45461</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O12" s="9" t="s">
         <v>170</v>
@@ -3558,10 +3558,10 @@
         <v>141</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>172</v>
@@ -3570,7 +3570,7 @@
         <v>45468</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="P13">
         <v>2024</v>
@@ -3587,7 +3587,7 @@
         <v>72</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>20</v>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>177</v>
@@ -3653,7 +3653,7 @@
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O15" s="9" t="s">
         <v>193</v>
@@ -3676,7 +3676,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>21</v>
@@ -3685,7 +3685,7 @@
         <v>194</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>133</v>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O16" s="9" t="s">
         <v>197</v>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>177</v>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O18" s="9" t="s">
         <v>202</v>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O19" s="9" t="s">
         <v>202</v>
@@ -3872,7 +3872,7 @@
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O20" s="9" t="s">
         <v>197</v>
@@ -3889,7 +3889,7 @@
         <v>71</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>17</v>
@@ -3901,7 +3901,7 @@
         <v>114</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="10" t="s">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O21" s="4" t="s">
         <v>177</v>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O22" s="9" t="s">
         <v>202</v>
@@ -4000,7 +4000,7 @@
         <v>45482</v>
       </c>
       <c r="N23" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O23" t="s">
         <v>193</v>
@@ -4017,7 +4017,7 @@
         <v>71</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>17</v>
@@ -4043,7 +4043,7 @@
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O24" s="9" t="s">
         <v>197</v>
@@ -4088,7 +4088,7 @@
         <v>45461</v>
       </c>
       <c r="N25" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O25" s="9" t="s">
         <v>170</v>
@@ -4131,7 +4131,7 @@
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>177</v>
@@ -4232,7 +4232,7 @@
         <v>8</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>72</v>
@@ -7902,7 +7902,7 @@
         <v>63</v>
       </c>
       <c r="G117" s="20" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H117" s="2" t="s">
         <v>139</v>

</xml_diff>